<commit_message>
Started working with HTML and CSS, created all files needed for all lessons
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TalTech\2. semester\IT süsteemide arendus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1ED470-F76C-489C-9DA1-C39EC26DDD23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAEFAD8-8252-4554-BB12-91EA8A7DD979}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Week 2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -93,6 +94,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Watching HTML and CSS course in MVA and writing notes</t>
   </si>
 </sst>
 </file>
@@ -449,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -556,6 +560,15 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -873,7 +886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -1291,4 +1304,360 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25C5994-C238-4873-A553-E9CBF31D311F}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="37.77734375" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="3.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="42"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="50"/>
+      <c r="C4" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="44">
+        <v>43498</v>
+      </c>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="45"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="48"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
+        <v>1</v>
+      </c>
+      <c r="B7" s="18">
+        <v>43501</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0.9375</v>
+      </c>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21">
+        <f>(D7-C7)*24*60 - E7</f>
+        <v>194.99999999999994</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="20"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5">
+        <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5">
+        <f>(D9-C9)*24*60 - E9</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5">
+        <f>(D10-C10)*24*60 - E10</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5">
+        <f>(D11-C11)*24*60 - E11</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5">
+        <f>(D12-C12)*24*60 - E12</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5">
+        <f>(D15-C15)*24*60 - E15</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="23">
+        <v>12</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="26"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="30">
+        <f>SUM(F7:F18)</f>
+        <v>194.99999999999994</v>
+      </c>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Lesson 3 finished log update
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAEFAD8-8252-4554-BB12-91EA8A7DD979}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD06821-7FBC-42EF-BC87-BD9DEA43AF01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -504,6 +504,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -560,15 +569,6 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -905,68 +905,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="42"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="43" t="s">
+      <c r="B4" s="53"/>
+      <c r="C4" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="44">
+      <c r="G4" s="47">
         <v>43498</v>
       </c>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="45"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="48"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="48"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1275,13 +1275,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="36"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>969.99999999999977</v>
@@ -1311,7 +1311,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1329,68 +1329,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="42"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="43" t="s">
+      <c r="B4" s="53"/>
+      <c r="C4" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="44">
+      <c r="G4" s="47">
         <v>43498</v>
       </c>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="45"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="48"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="48"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1427,17 +1427,19 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="D7" s="19">
-        <v>0.9375</v>
-      </c>
-      <c r="E7" s="20"/>
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E7" s="20">
+        <v>40</v>
+      </c>
       <c r="F7" s="21">
         <f>(D7-C7)*24*60 - E7</f>
-        <v>194.99999999999994</v>
+        <v>185</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="51" t="s">
+      <c r="H7" s="32" t="s">
         <v>21</v>
       </c>
       <c r="I7" s="20"/>
@@ -1447,7 +1449,9 @@
       <c r="A8" s="9">
         <v>2</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="7">
+        <v>43502</v>
+      </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="6"/>
@@ -1456,7 +1460,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="52"/>
+      <c r="H8" s="33"/>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
@@ -1490,7 +1494,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="H10" s="52"/>
+      <c r="H10" s="33"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
@@ -1507,7 +1511,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="6"/>
-      <c r="H11" s="52"/>
+      <c r="H11" s="33"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
@@ -1524,7 +1528,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="6"/>
-      <c r="H12" s="52"/>
+      <c r="H12" s="33"/>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
@@ -1541,7 +1545,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="6"/>
-      <c r="H13" s="52"/>
+      <c r="H13" s="33"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
@@ -1558,7 +1562,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="6"/>
-      <c r="H14" s="52"/>
+      <c r="H14" s="33"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
@@ -1575,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="6"/>
-      <c r="H15" s="52"/>
+      <c r="H15" s="33"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
@@ -1592,7 +1596,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="H16" s="52"/>
+      <c r="H16" s="33"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
@@ -1609,7 +1613,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="6"/>
-      <c r="H17" s="52"/>
+      <c r="H17" s="33"/>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
@@ -1626,21 +1630,21 @@
         <v>0</v>
       </c>
       <c r="G18" s="26"/>
-      <c r="H18" s="53"/>
+      <c r="H18" s="34"/>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="36"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>194.99999999999994</v>
+        <v>185</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>

</xml_diff>

<commit_message>
Lesson 5 and 6 finished Deleted "before" folders in lessons 2. 3 and 4 Log update
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD06821-7FBC-42EF-BC87-BD9DEA43AF01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D608BACB-86E0-4D90-81D9-E6E32C05A9CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -131,7 +131,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -449,11 +449,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -504,9 +541,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -569,6 +603,24 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -905,68 +957,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="43"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="46" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="47">
+      <c r="G4" s="46">
         <v>43498</v>
       </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="50"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1275,13 +1327,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>969.99999999999977</v>
@@ -1311,7 +1363,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1329,68 +1381,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="43"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="46" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="47">
+      <c r="G4" s="46">
         <v>43498</v>
       </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="50"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1416,7 +1468,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -1436,10 +1488,10 @@
         <f>(D7-C7)*24*60 - E7</f>
         <v>185</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="56" t="s">
         <v>21</v>
       </c>
       <c r="I7" s="20"/>
@@ -1452,15 +1504,19 @@
       <c r="B8" s="7">
         <v>43502</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="C8" s="8">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.60069444444444442</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="5">
         <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="33"/>
+        <v>34.999999999999872</v>
+      </c>
+      <c r="G8" s="54"/>
+      <c r="H8" s="57"/>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
@@ -1469,15 +1525,21 @@
         <v>3</v>
       </c>
       <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="6"/>
+      <c r="C9" s="8">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="E9" s="6">
+        <v>15</v>
+      </c>
       <c r="F9" s="5">
         <f>(D9-C9)*24*60 - E9</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="31"/>
+        <v>130.00000000000011</v>
+      </c>
+      <c r="G9" s="54"/>
+      <c r="H9" s="57"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
@@ -1493,8 +1555,8 @@
         <f>(D10-C10)*24*60 - E10</f>
         <v>0</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="33"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="58"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
@@ -1511,7 +1573,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="6"/>
-      <c r="H11" s="33"/>
+      <c r="H11" s="32"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
@@ -1528,7 +1590,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="6"/>
-      <c r="H12" s="33"/>
+      <c r="H12" s="32"/>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
@@ -1545,7 +1607,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="6"/>
-      <c r="H13" s="33"/>
+      <c r="H13" s="32"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
@@ -1562,7 +1624,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="6"/>
-      <c r="H14" s="33"/>
+      <c r="H14" s="32"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
@@ -1579,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="6"/>
-      <c r="H15" s="33"/>
+      <c r="H15" s="32"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
@@ -1596,7 +1658,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="H16" s="33"/>
+      <c r="H16" s="32"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
@@ -1613,7 +1675,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="6"/>
-      <c r="H17" s="33"/>
+      <c r="H17" s="32"/>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
@@ -1630,21 +1692,21 @@
         <v>0</v>
       </c>
       <c r="G18" s="26"/>
-      <c r="H18" s="34"/>
+      <c r="H18" s="33"/>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>185</v>
+        <v>350</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
@@ -1652,7 +1714,7 @@
       <c r="J19" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
@@ -1660,6 +1722,8 @@
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="G7:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Creating a webpage for a little practice
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1A4879-B451-4701-AC4E-FA8774A64DD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB6EA64-17F1-4EC3-8A89-279441BC9369}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Watching HTML and CSS course in MVA and writing notes</t>
+  </si>
+  <si>
+    <t>Reading HTML5 documentation and a little practice</t>
   </si>
 </sst>
 </file>
@@ -1385,7 +1388,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1686,20 +1689,30 @@
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>9</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="B15" s="7">
+        <v>43506</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.76041666666666663</v>
+      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="5">
         <f>(D15-C15)*24*60 - E15</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="32"/>
+        <v>54.999999999999964</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>22</v>
+      </c>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
@@ -1764,7 +1777,7 @@
       <c r="E19" s="38"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>885.00000000000045</v>
+        <v>940.00000000000045</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>

</xml_diff>

<commit_message>
Solution folder is organized into more intuitive folders(Solution update) Lesson 1 on JS Log update
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E180E81A-D602-4AAD-ABE5-1F5B44909220}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45C760B-15D0-4B4D-A2EC-D3ED1850D4FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
     <sheet name="Week 2" sheetId="3" r:id="rId2"/>
+    <sheet name="Week 3" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -100,6 +101,9 @@
   </si>
   <si>
     <t>Reading HTML5 documentation and a little practice</t>
+  </si>
+  <si>
+    <t>Watching JavaScript course and writing notes</t>
   </si>
 </sst>
 </file>
@@ -506,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -563,6 +567,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -620,6 +636,15 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -627,24 +652,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -982,68 +989,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="44"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="48"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="56"/>
+      <c r="C4" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="50">
         <v>43498</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="47"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="51"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="48"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="50"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="54"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="35"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1352,13 +1359,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="38"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="42"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>969.99999999999977</v>
@@ -1387,7 +1394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25C5994-C238-4873-A553-E9CBF31D311F}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1406,68 +1413,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="44"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="48"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="56"/>
+      <c r="C4" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="50">
         <v>43506</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="47"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="51"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="48"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="50"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="54"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="35"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1480,10 +1487,10 @@
       <c r="F6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="57" t="s">
+      <c r="H6" s="34" t="s">
         <v>9</v>
       </c>
       <c r="I6" s="14" t="s">
@@ -1513,10 +1520,10 @@
         <f>(D7-C7)*24*60 - E7</f>
         <v>185</v>
       </c>
-      <c r="G7" s="60" t="s">
+      <c r="G7" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="61" t="s">
+      <c r="H7" s="57" t="s">
         <v>21</v>
       </c>
       <c r="I7" s="20"/>
@@ -1540,8 +1547,8 @@
         <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
         <v>34.999999999999872</v>
       </c>
-      <c r="G8" s="53"/>
-      <c r="H8" s="55"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="62"/>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
@@ -1563,8 +1570,8 @@
         <f>(D9-C9)*24*60 - E9</f>
         <v>135.00000000000011</v>
       </c>
-      <c r="G9" s="53"/>
-      <c r="H9" s="55"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="62"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
@@ -1588,8 +1595,8 @@
         <f>(D10-C10)*24*60 - E10</f>
         <v>59.999999999999986</v>
       </c>
-      <c r="G10" s="53"/>
-      <c r="H10" s="55"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="62"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
@@ -1611,8 +1618,8 @@
         <f>(D11-C11)*24*60 - E11</f>
         <v>184.99999999999994</v>
       </c>
-      <c r="G11" s="53"/>
-      <c r="H11" s="55"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="62"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
@@ -1632,8 +1639,8 @@
         <f>(D12-C12)*24*60 - E12</f>
         <v>65.000000000000085</v>
       </c>
-      <c r="G12" s="54"/>
-      <c r="H12" s="56"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="58"/>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
@@ -1655,10 +1662,10 @@
         <f t="shared" si="0"/>
         <v>95.000000000000057</v>
       </c>
-      <c r="G13" s="58" t="s">
+      <c r="G13" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="59"/>
+      <c r="H13" s="36"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
@@ -1711,10 +1718,10 @@
         <f>(D15-C15)*24*60 - E15</f>
         <v>75.000000000000057</v>
       </c>
-      <c r="G15" s="60" t="s">
+      <c r="G15" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="61" t="s">
+      <c r="H15" s="57" t="s">
         <v>22</v>
       </c>
       <c r="I15" s="6"/>
@@ -1738,8 +1745,8 @@
         <f t="shared" si="0"/>
         <v>90.000000000000085</v>
       </c>
-      <c r="G16" s="54"/>
-      <c r="H16" s="56"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="58"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
@@ -1778,13 +1785,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="38"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="42"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>1050.0000000000005</v>
@@ -1811,4 +1818,368 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5305F5D1-E5D2-42C7-A8FE-5685192A2944}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="37.77734375" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="3.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="46"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="48"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="56"/>
+      <c r="C4" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="50">
+        <v>43506</v>
+      </c>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="51"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="54"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
+        <v>1</v>
+      </c>
+      <c r="B7" s="18">
+        <v>43507</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21">
+        <f>(D7-C7)*24*60 - E7</f>
+        <v>90</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="20"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7">
+        <v>43510</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5">
+        <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
+        <v>-975</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5">
+        <f>(D9-C9)*24*60 - E9</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="35"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5">
+        <f>(D10-C10)*24*60 - E10</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="35"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5">
+        <f>(D11-C11)*24*60 - E11</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5">
+        <f>(D12-C12)*24*60 - E12</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="35"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="35"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5">
+        <f>(D15-C15)*24*60 - E15</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="35"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="35"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="23">
+        <v>12</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="26"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="30">
+        <f>SUM(F7:F18)</f>
+        <v>-885</v>
+      </c>
+      <c r="G19" s="28"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Lesson 16 part 1 Log and solution update
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A910C86A-73F5-4B2B-95A2-0A6B5AE8B58D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196265A1-B45A-40FD-B60C-19528D511631}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1825,7 +1825,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H8" sqref="H8:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1957,7 +1957,7 @@
       <c r="I7" s="20"/>
       <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>2</v>
       </c>
@@ -1977,10 +1977,10 @@
         <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
         <v>279.99999999999983</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="57" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="6"/>
@@ -1990,16 +1990,24 @@
       <c r="A9" s="9">
         <v>3</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="6"/>
+      <c r="B9" s="7">
+        <v>43511</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="E9" s="6">
+        <v>80</v>
+      </c>
       <c r="F9" s="5">
         <f>(D9-C9)*24*60 - E9</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="36"/>
+        <v>140.00000000000003</v>
+      </c>
+      <c r="G9" s="60"/>
+      <c r="H9" s="62"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
@@ -2007,16 +2015,20 @@
       <c r="A10" s="9">
         <v>4</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="7">
+        <v>43512</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="6"/>
       <c r="F10" s="5">
         <f>(D10-C10)*24*60 - E10</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="36"/>
+        <v>-1020</v>
+      </c>
+      <c r="G10" s="60"/>
+      <c r="H10" s="62"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
@@ -2032,8 +2044,8 @@
         <f>(D11-C11)*24*60 - E11</f>
         <v>0</v>
       </c>
-      <c r="G11" s="35"/>
-      <c r="H11" s="36"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="58"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
@@ -2166,7 +2178,7 @@
       <c r="E19" s="42"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>369.99999999999983</v>
+        <v>-510.00000000000011</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>
@@ -2174,7 +2186,7 @@
       <c r="J19" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
@@ -2182,6 +2194,8 @@
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="H8:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Lessons 31 and 32
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46910E0-8726-45FD-8105-1943217A1CEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E317152C-7F99-4ADE-B826-906FB0AF8409}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2064,15 +2064,17 @@
       <c r="B12" s="7">
         <v>43513</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="8">
+        <v>0.90625</v>
+      </c>
       <c r="D12" s="8"/>
       <c r="E12" s="6"/>
       <c r="F12" s="5">
         <f>(D12-C12)*24*60 - E12</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="61"/>
-      <c r="H12" s="58"/>
+        <v>-1305</v>
+      </c>
+      <c r="G12" s="60"/>
+      <c r="H12" s="62"/>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
@@ -2088,8 +2090,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="35"/>
-      <c r="H13" s="36"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="58"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
@@ -2188,7 +2190,7 @@
       <c r="E19" s="42"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>769.99999999999989</v>
+        <v>-535.00000000000011</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>
@@ -2197,6 +2199,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="H8:H13"/>
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
@@ -2204,8 +2207,7 @@
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="G8:G12"/>
-    <mergeCell ref="H8:H12"/>
+    <mergeCell ref="G8:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished JavaScript course Solution and log update
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E317152C-7F99-4ADE-B826-906FB0AF8409}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE20A7DA-B3AF-4D34-9FCC-5CBA3B2CD74E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="24">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -1825,7 +1825,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2067,22 +2067,30 @@
       <c r="C12" s="8">
         <v>0.90625</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="8">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="E12" s="6"/>
       <c r="F12" s="5">
         <f>(D12-C12)*24*60 - E12</f>
-        <v>-1305</v>
+        <v>100.00000000000013</v>
       </c>
       <c r="G12" s="60"/>
       <c r="H12" s="62"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="10"/>
+      <c r="I12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="10">
+        <v>35</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>7</v>
       </c>
-      <c r="B13" s="7"/>
+      <c r="B13" s="7">
+        <v>43514</v>
+      </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
@@ -2090,8 +2098,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="61"/>
-      <c r="H13" s="58"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="36"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
@@ -2190,7 +2198,7 @@
       <c r="E19" s="42"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>-535.00000000000011</v>
+        <v>870</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>
@@ -2199,7 +2207,6 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="H8:H13"/>
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
@@ -2207,7 +2214,8 @@
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="G8:G12"/>
+    <mergeCell ref="H8:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Created project for MVC, first tasks completed
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA60C231-0981-49AA-897B-B2388D39B830}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E463E5F-ED3F-4908-8BB8-11969612743E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="28">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Reading "Clean Code"</t>
+  </si>
+  <si>
+    <t>Improving existing notes and writing notes on this weeks' lecture</t>
+  </si>
+  <si>
+    <t>Setting everything up for work with ASP.NET MVC Core (creating project, adding necessary components etc.) and completing first tasks</t>
   </si>
 </sst>
 </file>
@@ -1831,7 +1837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5305F5D1-E5D2-42C7-A8FE-5685192A2944}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:J5"/>
     </sheetView>
   </sheetViews>
@@ -2241,8 +2247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C8F448-C622-4990-958F-767F8A951C76}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:J5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2374,37 +2380,53 @@
       <c r="I7" s="20"/>
       <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>2</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="7">
+        <v>43516</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.95138888888888884</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="5">
         <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="35"/>
-      <c r="H8" s="36"/>
+        <v>49.999999999999986</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>26</v>
+      </c>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>3</v>
       </c>
       <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="C9" s="8">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="E9" s="6"/>
       <c r="F9" s="5">
         <f>(D9-C9)*24*60 - E9</f>
-        <v>0</v>
+        <v>30.000000000000053</v>
       </c>
       <c r="G9" s="35"/>
-      <c r="H9" s="36"/>
+      <c r="H9" s="36" t="s">
+        <v>27</v>
+      </c>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
@@ -2571,7 +2593,7 @@
       <c r="E19" s="42"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>90</v>
+        <v>170.00000000000006</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>

</xml_diff>

<commit_message>
Upgarded project to .NET Core 2.2 Labor 2, installed and updated necessary packages Log update
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E463E5F-ED3F-4908-8BB8-11969612743E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E3F5FB-7BFB-4A9F-A84F-78751A523909}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="29">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Setting everything up for work with ASP.NET MVC Core (creating project, adding necessary components etc.) and completing first tasks</t>
+  </si>
+  <si>
+    <t>Completing homework on UI/UX</t>
   </si>
 </sst>
 </file>
@@ -2248,7 +2251,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2423,7 +2426,9 @@
         <f>(D9-C9)*24*60 - E9</f>
         <v>30.000000000000053</v>
       </c>
-      <c r="G9" s="35"/>
+      <c r="G9" s="35" t="s">
+        <v>16</v>
+      </c>
       <c r="H9" s="36" t="s">
         <v>27</v>
       </c>
@@ -2434,16 +2439,26 @@
       <c r="A10" s="9">
         <v>4</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="7">
+        <v>43517</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.73611111111111116</v>
+      </c>
       <c r="E10" s="6"/>
       <c r="F10" s="5">
         <f>(D10-C10)*24*60 - E10</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="36"/>
+        <v>85.000000000000014</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>28</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
@@ -2451,15 +2466,23 @@
       <c r="A11" s="9">
         <v>5</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="B11" s="7">
+        <v>43518</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="E11" s="6"/>
       <c r="F11" s="5">
         <f>(D11-C11)*24*60 - E11</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="35"/>
+        <v>120.00000000000006</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>12</v>
+      </c>
       <c r="H11" s="36"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
@@ -2469,12 +2492,14 @@
         <v>6</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
+      <c r="C12" s="8">
+        <v>0.70138888888888884</v>
+      </c>
       <c r="D12" s="8"/>
       <c r="E12" s="6"/>
       <c r="F12" s="5">
         <f>(D12-C12)*24*60 - E12</f>
-        <v>0</v>
+        <v>-1009.9999999999999</v>
       </c>
       <c r="G12" s="35"/>
       <c r="H12" s="36"/>
@@ -2593,7 +2618,7 @@
       <c r="E19" s="42"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>170.00000000000006</v>
+        <v>-634.99999999999977</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>

</xml_diff>

<commit_message>
Labor 25 (Save not working)
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3D9B88-C0A9-429A-B391-D88711B15486}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81085A2-BB50-4480-B70C-82019447B0E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2255,7 +2255,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:J5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2578,11 +2578,13 @@
       <c r="C15" s="8">
         <v>0.93402777777777779</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="8">
+        <v>0.98611111111111116</v>
+      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="5">
         <f>(D15-C15)*24*60 - E15</f>
-        <v>-1345</v>
+        <v>75.000000000000057</v>
       </c>
       <c r="G15" s="61"/>
       <c r="H15" s="58"/>
@@ -2650,7 +2652,7 @@
       <c r="E19" s="42"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>-39.999999999999545</v>
+        <v>1380.0000000000005</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>

</xml_diff>

<commit_message>
Get Started part 1
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5290890A-BB81-490B-A3FE-F3FC229B1BFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664DFBDF-B6F0-409A-917D-08F71F4FCE85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Week 3" sheetId="5" r:id="rId3"/>
     <sheet name="Week 4" sheetId="6" r:id="rId4"/>
     <sheet name="Week 5" sheetId="7" r:id="rId5"/>
+    <sheet name="Week 6" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="35">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -136,6 +137,9 @@
   </si>
   <si>
     <t>Finishing MVC homewrok</t>
+  </si>
+  <si>
+    <t>Completing MVC with EF Core homework</t>
   </si>
 </sst>
 </file>
@@ -2693,7 +2697,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2912,13 +2916,15 @@
       <c r="C11" s="8">
         <v>0.82986111111111116</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="8">
+        <v>0.875</v>
+      </c>
       <c r="E11" s="6">
         <v>10</v>
       </c>
       <c r="F11" s="5">
         <f>(D11-C11)*24*60 - E11</f>
-        <v>-1205</v>
+        <v>54.999999999999929</v>
       </c>
       <c r="G11" s="35" t="s">
         <v>16</v>
@@ -2926,6 +2932,358 @@
       <c r="H11" s="36" t="s">
         <v>33</v>
       </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8">
+        <v>0.93402777777777779</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5">
+        <f>(D12-C12)*24*60 - E12</f>
+        <v>-1345</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5">
+        <f>(D15-C15)*24*60 - E15</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="35"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="35"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="23">
+        <v>12</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="26"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="30">
+        <f>SUM(F7:F18)</f>
+        <v>-844.99999999999977</v>
+      </c>
+      <c r="G19" s="28"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793231FC-74F6-4F49-92E7-8F29249865E3}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="41.6640625" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="3.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="46"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="48"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="56"/>
+      <c r="C4" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="50">
+        <v>43534</v>
+      </c>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="51"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="54"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
+        <v>1</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21">
+        <f>(D7-C7)*24*60 - E7</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="35"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5">
+        <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="35"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5">
+        <f>(D9-C9)*24*60 - E9</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="35"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5">
+        <f>(D10-C10)*24*60 - E10</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="35"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5">
+        <f>(D11-C11)*24*60 - E11</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
@@ -3058,7 +3416,7 @@
       <c r="E19" s="42"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>-759.99999999999977</v>
+        <v>0</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>

</xml_diff>

<commit_message>
Sort, filter, page, and group
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59150793-41B1-413B-8AE6-BF7C9F226CEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB21928B-7B76-4753-A605-33AE40AB950E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2697,7 +2697,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2996,10 +2996,12 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="D14" s="8"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="6">
+        <v>10</v>
+      </c>
       <c r="F14" s="5">
         <f t="shared" si="0"/>
-        <v>-615</v>
+        <v>-625</v>
       </c>
       <c r="G14" s="61"/>
       <c r="H14" s="61"/>
@@ -3084,7 +3086,7 @@
       <c r="E19" s="42"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>

</xml_diff>

<commit_message>
Create a complex data model
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB21928B-7B76-4753-A605-33AE40AB950E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966C1C60-1F72-478D-AF63-B3EA161CC2BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="35">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -2430,7 +2430,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>3</v>
       </c>
@@ -2697,7 +2697,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2995,16 +2995,18 @@
       <c r="C14" s="8">
         <v>0.42708333333333331</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="8">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="E14" s="6">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="0"/>
-        <v>-625</v>
-      </c>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
+        <v>95.000000000000085</v>
+      </c>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
@@ -3013,15 +3015,19 @@
         <v>9</v>
       </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="8">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.60069444444444442</v>
+      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="5">
         <f>(D15-C15)*24*60 - E15</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="35"/>
-      <c r="H15" s="36"/>
+        <v>45</v>
+      </c>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
@@ -3030,15 +3036,23 @@
         <v>10</v>
       </c>
       <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="C16" s="8">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="35"/>
-      <c r="H16" s="36"/>
+        <v>90</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>13</v>
+      </c>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
@@ -3047,15 +3061,21 @@
         <v>11</v>
       </c>
       <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8">
+        <v>0.90972222222222221</v>
+      </c>
       <c r="D17" s="8"/>
       <c r="E17" s="6"/>
       <c r="F17" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="32"/>
+        <v>-1310</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>34</v>
+      </c>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
@@ -3086,7 +3106,7 @@
       <c r="E19" s="42"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>-15</v>
+        <v>-469.99999999999989</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>
@@ -3102,8 +3122,8 @@
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H12:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
@@ -3115,7 +3135,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Razor Pages 1.1 - Get Started
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA55EA04-1956-4B1D-800F-F53716FEB2C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1751AE1D-A0F5-4164-B462-C883FFB7C8BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Week 4" sheetId="6" r:id="rId4"/>
     <sheet name="Week 5" sheetId="7" r:id="rId5"/>
     <sheet name="Week 6" sheetId="8" r:id="rId6"/>
+    <sheet name="Week 7" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="44">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -155,6 +156,18 @@
   </si>
   <si>
     <t>Watching Martin Fowleri ja Robert Martini videod</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>Helping others with homework</t>
+  </si>
+  <si>
+    <t>Prep</t>
+  </si>
+  <si>
+    <t>Completing "Get started with Razor pages" project</t>
   </si>
 </sst>
 </file>
@@ -561,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -704,6 +717,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1021,25 +1052,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="41.6640625" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" customWidth="1"/>
-    <col min="10" max="10" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
@@ -1053,7 +1082,7 @@
       <c r="I2" s="44"/>
       <c r="J2" s="45"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="46"/>
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
@@ -1065,7 +1094,7 @@
       <c r="I3" s="47"/>
       <c r="J3" s="48"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="55" t="s">
         <v>1</v>
       </c>
@@ -1085,7 +1114,7 @@
       <c r="I4" s="50"/>
       <c r="J4" s="51"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="52"/>
       <c r="B5" s="53"/>
       <c r="C5" s="53"/>
@@ -1097,7 +1126,7 @@
       <c r="I5" s="53"/>
       <c r="J5" s="54"/>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="38" t="s">
         <v>3</v>
       </c>
@@ -1127,7 +1156,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -1145,7 +1174,7 @@
         <f>(D7-C7)*24*60 - E7</f>
         <v>90</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="67" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="20" t="s">
@@ -1154,7 +1183,7 @@
       <c r="I7" s="20"/>
       <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>2</v>
       </c>
@@ -1170,7 +1199,7 @@
         <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
         <v>19.999999999999929</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="66" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -1179,7 +1208,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>3</v>
       </c>
@@ -1195,7 +1224,7 @@
         <f>(D9-C9)*24*60 - E9</f>
         <v>29.999999999999893</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="66" t="s">
         <v>16</v>
       </c>
       <c r="H9" s="31" t="s">
@@ -1204,7 +1233,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>4</v>
       </c>
@@ -1222,7 +1251,7 @@
         <f>(D10-C10)*24*60 - E10</f>
         <v>90</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="66" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="6" t="s">
@@ -1231,7 +1260,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>5</v>
       </c>
@@ -1249,7 +1278,7 @@
         <f>(D11-C11)*24*60 - E11</f>
         <v>114.99999999999999</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="66" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="6" t="s">
@@ -1258,7 +1287,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>6</v>
       </c>
@@ -1274,7 +1303,7 @@
         <f>(D12-C12)*24*60 - E12</f>
         <v>189.99999999999997</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="66" t="s">
         <v>16</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -1283,7 +1312,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>7</v>
       </c>
@@ -1301,14 +1330,14 @@
         <f t="shared" si="0"/>
         <v>170.00000000000003</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="66" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>8</v>
       </c>
@@ -1328,7 +1357,7 @@
         <f t="shared" si="0"/>
         <v>265</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="66" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="6" t="s">
@@ -1341,7 +1370,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>9</v>
       </c>
@@ -1353,12 +1382,12 @@
         <f>(D15-C15)*24*60 - E15</f>
         <v>0</v>
       </c>
-      <c r="G15" s="6"/>
+      <c r="G15" s="66"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>10</v>
       </c>
@@ -1370,12 +1399,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="6"/>
+      <c r="G16" s="66"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>11</v>
       </c>
@@ -1387,12 +1416,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="6"/>
+      <c r="G17" s="66"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>12</v>
       </c>
@@ -1404,12 +1433,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="26"/>
+      <c r="G18" s="68"/>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="40" t="s">
         <v>14</v>
       </c>
@@ -1445,25 +1474,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25C5994-C238-4873-A553-E9CBF31D311F}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="41.6640625" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" customWidth="1"/>
-    <col min="10" max="10" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
@@ -1477,7 +1504,7 @@
       <c r="I2" s="44"/>
       <c r="J2" s="45"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="46"/>
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
@@ -1489,7 +1516,7 @@
       <c r="I3" s="47"/>
       <c r="J3" s="48"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="55" t="s">
         <v>1</v>
       </c>
@@ -1509,7 +1536,7 @@
       <c r="I4" s="50"/>
       <c r="J4" s="51"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="52"/>
       <c r="B5" s="53"/>
       <c r="C5" s="53"/>
@@ -1521,7 +1548,7 @@
       <c r="I5" s="53"/>
       <c r="J5" s="54"/>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="38" t="s">
         <v>3</v>
       </c>
@@ -1551,7 +1578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -1580,7 +1607,7 @@
       <c r="I7" s="20"/>
       <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>2</v>
       </c>
@@ -1603,7 +1630,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>3</v>
       </c>
@@ -1626,7 +1653,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>4</v>
       </c>
@@ -1651,7 +1678,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>5</v>
       </c>
@@ -1674,7 +1701,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>6</v>
       </c>
@@ -1695,7 +1722,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>7</v>
       </c>
@@ -1713,14 +1740,14 @@
         <f t="shared" si="0"/>
         <v>95.000000000000057</v>
       </c>
-      <c r="G13" s="35" t="s">
+      <c r="G13" s="65" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="36"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>8</v>
       </c>
@@ -1738,7 +1765,7 @@
         <f t="shared" si="0"/>
         <v>125.0000000000002</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="66" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="32" t="s">
@@ -1751,7 +1778,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>9</v>
       </c>
@@ -1778,7 +1805,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>10</v>
       </c>
@@ -1801,7 +1828,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>11</v>
       </c>
@@ -1813,12 +1840,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="6"/>
+      <c r="G17" s="66"/>
       <c r="H17" s="32"/>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>12</v>
       </c>
@@ -1830,12 +1857,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="26"/>
+      <c r="G18" s="68"/>
       <c r="H18" s="33"/>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="40" t="s">
         <v>14</v>
       </c>
@@ -1875,25 +1902,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5305F5D1-E5D2-42C7-A8FE-5685192A2944}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:J5"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="41.6640625" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" customWidth="1"/>
-    <col min="10" max="10" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
@@ -1907,7 +1932,7 @@
       <c r="I2" s="44"/>
       <c r="J2" s="45"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="46"/>
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
@@ -1919,7 +1944,7 @@
       <c r="I3" s="47"/>
       <c r="J3" s="48"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="55" t="s">
         <v>1</v>
       </c>
@@ -1939,7 +1964,7 @@
       <c r="I4" s="50"/>
       <c r="J4" s="51"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="52"/>
       <c r="B5" s="53"/>
       <c r="C5" s="53"/>
@@ -1951,7 +1976,7 @@
       <c r="I5" s="53"/>
       <c r="J5" s="54"/>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="38" t="s">
         <v>3</v>
       </c>
@@ -1981,7 +2006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -1999,7 +2024,7 @@
         <f>(D7-C7)*24*60 - E7</f>
         <v>90</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="65" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="36" t="s">
@@ -2008,7 +2033,7 @@
       <c r="I7" s="20"/>
       <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>2</v>
       </c>
@@ -2037,7 +2062,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>3</v>
       </c>
@@ -2062,7 +2087,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>4</v>
       </c>
@@ -2087,7 +2112,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>5</v>
       </c>
@@ -2108,7 +2133,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>6</v>
       </c>
@@ -2135,7 +2160,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>7</v>
       </c>
@@ -2153,7 +2178,7 @@
         <f t="shared" si="0"/>
         <v>135.00000000000009</v>
       </c>
-      <c r="G13" s="35" t="s">
+      <c r="G13" s="65" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="36" t="s">
@@ -2162,7 +2187,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>8</v>
       </c>
@@ -2174,12 +2199,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="6"/>
+      <c r="G14" s="66"/>
       <c r="H14" s="32"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>9</v>
       </c>
@@ -2191,12 +2216,12 @@
         <f>(D15-C15)*24*60 - E15</f>
         <v>0</v>
       </c>
-      <c r="G15" s="35"/>
+      <c r="G15" s="65"/>
       <c r="H15" s="36"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>10</v>
       </c>
@@ -2208,12 +2233,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="35"/>
+      <c r="G16" s="65"/>
       <c r="H16" s="36"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>11</v>
       </c>
@@ -2225,12 +2250,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="6"/>
+      <c r="G17" s="66"/>
       <c r="H17" s="32"/>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>12</v>
       </c>
@@ -2242,12 +2267,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="26"/>
+      <c r="G18" s="68"/>
       <c r="H18" s="32"/>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="40" t="s">
         <v>14</v>
       </c>
@@ -2285,25 +2310,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C8F448-C622-4990-958F-767F8A951C76}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="41.6640625" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" customWidth="1"/>
-    <col min="10" max="10" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
@@ -2317,7 +2340,7 @@
       <c r="I2" s="44"/>
       <c r="J2" s="45"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="46"/>
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
@@ -2329,7 +2352,7 @@
       <c r="I3" s="47"/>
       <c r="J3" s="48"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="55" t="s">
         <v>1</v>
       </c>
@@ -2349,7 +2372,7 @@
       <c r="I4" s="50"/>
       <c r="J4" s="51"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="52"/>
       <c r="B5" s="53"/>
       <c r="C5" s="53"/>
@@ -2361,7 +2384,7 @@
       <c r="I5" s="53"/>
       <c r="J5" s="54"/>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="38" t="s">
         <v>3</v>
       </c>
@@ -2391,7 +2414,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -2409,7 +2432,7 @@
         <f>(D7-C7)*24*60 - E7</f>
         <v>90</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="65" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="36" t="s">
@@ -2418,7 +2441,7 @@
       <c r="I7" s="20"/>
       <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>2</v>
       </c>
@@ -2436,7 +2459,7 @@
         <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
         <v>49.999999999999986</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="65" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="36" t="s">
@@ -2445,7 +2468,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>3</v>
       </c>
@@ -2461,7 +2484,7 @@
         <f>(D9-C9)*24*60 - E9</f>
         <v>30.000000000000053</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="65" t="s">
         <v>16</v>
       </c>
       <c r="H9" s="36" t="s">
@@ -2470,7 +2493,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>4</v>
       </c>
@@ -2488,7 +2511,7 @@
         <f>(D10-C10)*24*60 - E10</f>
         <v>85.000000000000014</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="65" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="36" t="s">
@@ -2497,7 +2520,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>5</v>
       </c>
@@ -2515,14 +2538,14 @@
         <f>(D11-C11)*24*60 - E11</f>
         <v>120.00000000000006</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="65" t="s">
         <v>12</v>
       </c>
       <c r="H11" s="36"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>6</v>
       </c>
@@ -2549,7 +2572,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>7</v>
       </c>
@@ -2574,7 +2597,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>8</v>
       </c>
@@ -2599,7 +2622,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>9</v>
       </c>
@@ -2622,7 +2645,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>10</v>
       </c>
@@ -2634,12 +2657,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="35"/>
+      <c r="G16" s="65"/>
       <c r="H16" s="36"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>11</v>
       </c>
@@ -2651,12 +2674,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="6"/>
+      <c r="G17" s="66"/>
       <c r="H17" s="32"/>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>12</v>
       </c>
@@ -2668,12 +2691,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="26"/>
+      <c r="G18" s="68"/>
       <c r="H18" s="32"/>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="40" t="s">
         <v>14</v>
       </c>
@@ -2711,25 +2734,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5BDBD6A-C2F2-457B-9BFA-ED9D1059E940}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="41.6640625" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" customWidth="1"/>
-    <col min="10" max="10" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
@@ -2743,7 +2764,7 @@
       <c r="I2" s="44"/>
       <c r="J2" s="45"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="46"/>
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
@@ -2755,7 +2776,7 @@
       <c r="I3" s="47"/>
       <c r="J3" s="48"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="55" t="s">
         <v>1</v>
       </c>
@@ -2775,7 +2796,7 @@
       <c r="I4" s="50"/>
       <c r="J4" s="51"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="52"/>
       <c r="B5" s="53"/>
       <c r="C5" s="53"/>
@@ -2787,7 +2808,7 @@
       <c r="I5" s="53"/>
       <c r="J5" s="54"/>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="38" t="s">
         <v>3</v>
       </c>
@@ -2817,7 +2838,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -2835,14 +2856,14 @@
         <f>(D7-C7)*24*60 - E7</f>
         <v>151.00000000000011</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="65" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="36"/>
       <c r="I7" s="20"/>
       <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>2</v>
       </c>
@@ -2858,7 +2879,7 @@
         <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
         <v>48.999999999999986</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="65" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="36" t="s">
@@ -2867,7 +2888,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>3</v>
       </c>
@@ -2885,8 +2906,8 @@
         <f>(D9-C9)*24*60 - E9</f>
         <v>130.00000000000009</v>
       </c>
-      <c r="G9" s="35" t="s">
-        <v>16</v>
+      <c r="G9" s="65" t="s">
+        <v>24</v>
       </c>
       <c r="H9" s="36" t="s">
         <v>31</v>
@@ -2894,7 +2915,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>4</v>
       </c>
@@ -2914,7 +2935,7 @@
         <f>(D10-C10)*24*60 - E10</f>
         <v>114.99999999999997</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="65" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="36" t="s">
@@ -2923,7 +2944,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>5</v>
       </c>
@@ -2941,7 +2962,7 @@
         <f>(D11-C11)*24*60 - E11</f>
         <v>54.999999999999929</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="65" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="36" t="s">
@@ -2954,7 +2975,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>6</v>
       </c>
@@ -2979,7 +3000,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>7</v>
       </c>
@@ -3004,7 +3025,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>8</v>
       </c>
@@ -3029,7 +3050,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>9</v>
       </c>
@@ -3050,7 +3071,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>10</v>
       </c>
@@ -3066,7 +3087,7 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="G16" s="35" t="s">
+      <c r="G16" s="65" t="s">
         <v>12</v>
       </c>
       <c r="H16" s="35" t="s">
@@ -3075,7 +3096,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>11</v>
       </c>
@@ -3091,7 +3112,7 @@
         <f t="shared" si="0"/>
         <v>120.00000000000006</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="66" t="s">
         <v>16</v>
       </c>
       <c r="H17" s="32" t="s">
@@ -3100,7 +3121,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>12</v>
       </c>
@@ -3112,12 +3133,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="26"/>
+      <c r="G18" s="68"/>
       <c r="H18" s="32"/>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="40" t="s">
         <v>14</v>
       </c>
@@ -3155,25 +3176,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793231FC-74F6-4F49-92E7-8F29249865E3}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="47.5546875" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" customWidth="1"/>
-    <col min="10" max="10" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
@@ -3187,7 +3206,7 @@
       <c r="I2" s="44"/>
       <c r="J2" s="45"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="46"/>
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
@@ -3199,7 +3218,7 @@
       <c r="I3" s="47"/>
       <c r="J3" s="48"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="55" t="s">
         <v>1</v>
       </c>
@@ -3219,7 +3238,7 @@
       <c r="I4" s="50"/>
       <c r="J4" s="51"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="52"/>
       <c r="B5" s="53"/>
       <c r="C5" s="53"/>
@@ -3231,7 +3250,7 @@
       <c r="I5" s="53"/>
       <c r="J5" s="54"/>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="38" t="s">
         <v>3</v>
       </c>
@@ -3261,7 +3280,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -3279,7 +3298,7 @@
         <f>(D7-C7)*24*60 - E7</f>
         <v>205.00000000000006</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="65" t="s">
         <v>16</v>
       </c>
       <c r="H7" s="32" t="s">
@@ -3288,7 +3307,7 @@
       <c r="I7" s="20"/>
       <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>2</v>
       </c>
@@ -3306,7 +3325,7 @@
         <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
         <v>59.999999999999943</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="65" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="36" t="s">
@@ -3315,7 +3334,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>3</v>
       </c>
@@ -3331,8 +3350,8 @@
         <f>(D9-C9)*24*60 - E9</f>
         <v>49.999999999999986</v>
       </c>
-      <c r="G9" s="35" t="s">
-        <v>16</v>
+      <c r="G9" s="65" t="s">
+        <v>24</v>
       </c>
       <c r="H9" s="36" t="s">
         <v>37</v>
@@ -3340,7 +3359,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>4</v>
       </c>
@@ -3358,14 +3377,14 @@
         <f>(D10-C10)*24*60 - E10</f>
         <v>140.00000000000006</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="65" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="36"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>5</v>
       </c>
@@ -3383,7 +3402,7 @@
         <f>(D11-C11)*24*60 - E11</f>
         <v>129.99999999999994</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="65" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="36" t="s">
@@ -3394,7 +3413,7 @@
       </c>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>6</v>
       </c>
@@ -3412,8 +3431,8 @@
         <f>(D12-C12)*24*60 - E12</f>
         <v>190.00000000000017</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>16</v>
+      <c r="G12" s="66" t="s">
+        <v>24</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>37</v>
@@ -3421,7 +3440,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>7</v>
       </c>
@@ -3437,8 +3456,8 @@
         <f t="shared" si="0"/>
         <v>35.000000000000036</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>16</v>
+      <c r="G13" s="66" t="s">
+        <v>40</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>38</v>
@@ -3446,7 +3465,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>8</v>
       </c>
@@ -3463,15 +3482,15 @@
         <v>150.00000000000011</v>
       </c>
       <c r="G14" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="63" t="s">
         <v>37</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>9</v>
       </c>
@@ -3490,11 +3509,11 @@
         <v>94.999999999999986</v>
       </c>
       <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
+      <c r="H15" s="64"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>10</v>
       </c>
@@ -3512,16 +3531,18 @@
         <f t="shared" si="0"/>
         <v>59.999999999999744</v>
       </c>
-      <c r="G16" s="35" t="s">
+      <c r="G16" s="65" t="s">
         <v>16</v>
       </c>
       <c r="H16" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I16" s="6"/>
+      <c r="I16" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>11</v>
       </c>
@@ -3533,12 +3554,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="6"/>
+      <c r="G17" s="66"/>
       <c r="H17" s="32"/>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>12</v>
       </c>
@@ -3550,12 +3571,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="26"/>
+      <c r="G18" s="68"/>
       <c r="H18" s="32"/>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="40" t="s">
         <v>14</v>
       </c>
@@ -3587,4 +3608,406 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4F9FF2-393D-4BE8-8309-82E6CF37137A}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="46"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="48"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="56"/>
+      <c r="C4" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="50">
+        <v>43541</v>
+      </c>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="51"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="54"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>1</v>
+      </c>
+      <c r="B7" s="18">
+        <v>43535</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21">
+        <f>(D7-C7)*24*60 - E7</f>
+        <v>90</v>
+      </c>
+      <c r="G7" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="20"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7">
+        <v>43536</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5">
+        <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
+        <v>20.000000000000249</v>
+      </c>
+      <c r="G8" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7">
+        <v>43538</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5">
+        <f>(D9-C9)*24*60 - E9</f>
+        <v>84.999999999999858</v>
+      </c>
+      <c r="G9" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8">
+        <v>0.90625</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5">
+        <f>(D10-C10)*24*60 - E10</f>
+        <v>30.000000000000053</v>
+      </c>
+      <c r="G10" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7">
+        <v>43539</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5">
+        <f>(D11-C11)*24*60 - E11</f>
+        <v>20.000000000000089</v>
+      </c>
+      <c r="G11" s="61"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7">
+        <v>43540</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5">
+        <f>(D12-C12)*24*60 - E12</f>
+        <v>-755</v>
+      </c>
+      <c r="G12" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="61"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="65"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5">
+        <f>(D15-C15)*24*60 - E15</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="65"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="65"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="66"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="23">
+        <v>12</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="68"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="30">
+        <f>SUM(F7:F18)</f>
+        <v>-509.99999999999977</v>
+      </c>
+      <c r="G19" s="28"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Razor Pages 1.2.1 - Minor fix
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1751AE1D-A0F5-4164-B462-C883FFB7C8BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399D54F1-3DFC-4D6E-A063-22FFFDCEA195}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -643,6 +643,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -723,18 +735,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1069,68 +1069,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="49" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="50">
+      <c r="G4" s="54">
         <v>43498</v>
       </c>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="51"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="54"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1174,7 +1174,7 @@
         <f>(D7-C7)*24*60 - E7</f>
         <v>90</v>
       </c>
-      <c r="G7" s="67" t="s">
+      <c r="G7" s="40" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="20" t="s">
@@ -1199,7 +1199,7 @@
         <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
         <v>19.999999999999929</v>
       </c>
-      <c r="G8" s="66" t="s">
+      <c r="G8" s="39" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -1224,7 +1224,7 @@
         <f>(D9-C9)*24*60 - E9</f>
         <v>29.999999999999893</v>
       </c>
-      <c r="G9" s="66" t="s">
+      <c r="G9" s="39" t="s">
         <v>16</v>
       </c>
       <c r="H9" s="31" t="s">
@@ -1251,7 +1251,7 @@
         <f>(D10-C10)*24*60 - E10</f>
         <v>90</v>
       </c>
-      <c r="G10" s="66" t="s">
+      <c r="G10" s="39" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="6" t="s">
@@ -1278,7 +1278,7 @@
         <f>(D11-C11)*24*60 - E11</f>
         <v>114.99999999999999</v>
       </c>
-      <c r="G11" s="66" t="s">
+      <c r="G11" s="39" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="6" t="s">
@@ -1303,7 +1303,7 @@
         <f>(D12-C12)*24*60 - E12</f>
         <v>189.99999999999997</v>
       </c>
-      <c r="G12" s="66" t="s">
+      <c r="G12" s="39" t="s">
         <v>16</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -1330,7 +1330,7 @@
         <f t="shared" si="0"/>
         <v>170.00000000000003</v>
       </c>
-      <c r="G13" s="66" t="s">
+      <c r="G13" s="39" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="6"/>
@@ -1357,7 +1357,7 @@
         <f t="shared" si="0"/>
         <v>265</v>
       </c>
-      <c r="G14" s="66" t="s">
+      <c r="G14" s="39" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="6" t="s">
@@ -1382,7 +1382,7 @@
         <f>(D15-C15)*24*60 - E15</f>
         <v>0</v>
       </c>
-      <c r="G15" s="66"/>
+      <c r="G15" s="39"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
@@ -1399,7 +1399,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="66"/>
+      <c r="G16" s="39"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
@@ -1416,7 +1416,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="66"/>
+      <c r="G17" s="39"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
@@ -1433,19 +1433,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="68"/>
+      <c r="G18" s="41"/>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>969.99999999999977</v>
@@ -1491,68 +1491,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="49" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="50">
+      <c r="G4" s="54">
         <v>43506</v>
       </c>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="51"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="54"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1598,10 +1598,10 @@
         <f>(D7-C7)*24*60 - E7</f>
         <v>185</v>
       </c>
-      <c r="G7" s="59" t="s">
+      <c r="G7" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="57" t="s">
+      <c r="H7" s="61" t="s">
         <v>21</v>
       </c>
       <c r="I7" s="20"/>
@@ -1625,8 +1625,8 @@
         <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
         <v>34.999999999999872</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="62"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="66"/>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
@@ -1648,8 +1648,8 @@
         <f>(D9-C9)*24*60 - E9</f>
         <v>135.00000000000011</v>
       </c>
-      <c r="G9" s="60"/>
-      <c r="H9" s="62"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="66"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
@@ -1673,8 +1673,8 @@
         <f>(D10-C10)*24*60 - E10</f>
         <v>59.999999999999986</v>
       </c>
-      <c r="G10" s="60"/>
-      <c r="H10" s="62"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="66"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
@@ -1696,8 +1696,8 @@
         <f>(D11-C11)*24*60 - E11</f>
         <v>184.99999999999994</v>
       </c>
-      <c r="G11" s="60"/>
-      <c r="H11" s="62"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="66"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
@@ -1717,8 +1717,8 @@
         <f>(D12-C12)*24*60 - E12</f>
         <v>65.000000000000085</v>
       </c>
-      <c r="G12" s="61"/>
-      <c r="H12" s="58"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="62"/>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
@@ -1740,7 +1740,7 @@
         <f t="shared" si="0"/>
         <v>95.000000000000057</v>
       </c>
-      <c r="G13" s="65" t="s">
+      <c r="G13" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="36"/>
@@ -1765,7 +1765,7 @@
         <f t="shared" si="0"/>
         <v>125.0000000000002</v>
       </c>
-      <c r="G14" s="66" t="s">
+      <c r="G14" s="39" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="32" t="s">
@@ -1796,10 +1796,10 @@
         <f>(D15-C15)*24*60 - E15</f>
         <v>75.000000000000057</v>
       </c>
-      <c r="G15" s="59" t="s">
+      <c r="G15" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="57" t="s">
+      <c r="H15" s="61" t="s">
         <v>22</v>
       </c>
       <c r="I15" s="6"/>
@@ -1823,8 +1823,8 @@
         <f t="shared" si="0"/>
         <v>90.000000000000085</v>
       </c>
-      <c r="G16" s="61"/>
-      <c r="H16" s="58"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="62"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
@@ -1840,7 +1840,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="66"/>
+      <c r="G17" s="39"/>
       <c r="H17" s="32"/>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
@@ -1857,19 +1857,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="68"/>
+      <c r="G18" s="41"/>
       <c r="H18" s="33"/>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>1050.0000000000005</v>
@@ -1919,68 +1919,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="49" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="50">
+      <c r="G4" s="54">
         <v>43514</v>
       </c>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="51"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="54"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2024,7 +2024,7 @@
         <f>(D7-C7)*24*60 - E7</f>
         <v>90</v>
       </c>
-      <c r="G7" s="65" t="s">
+      <c r="G7" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="36" t="s">
@@ -2053,10 +2053,10 @@
         <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
         <v>279.99999999999983</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="57" t="s">
+      <c r="H8" s="61" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="6"/>
@@ -2082,8 +2082,8 @@
         <f>(D9-C9)*24*60 - E9</f>
         <v>140.00000000000003</v>
       </c>
-      <c r="G9" s="60"/>
-      <c r="H9" s="62"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="66"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
@@ -2107,8 +2107,8 @@
         <f>(D10-C10)*24*60 - E10</f>
         <v>145.00000000000006</v>
       </c>
-      <c r="G10" s="60"/>
-      <c r="H10" s="62"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="66"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
@@ -2128,8 +2128,8 @@
         <f>(D11-C11)*24*60 - E11</f>
         <v>114.99999999999991</v>
       </c>
-      <c r="G11" s="60"/>
-      <c r="H11" s="62"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="66"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
@@ -2151,8 +2151,8 @@
         <f>(D12-C12)*24*60 - E12</f>
         <v>100.00000000000013</v>
       </c>
-      <c r="G12" s="60"/>
-      <c r="H12" s="62"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="66"/>
       <c r="I12" s="6" t="s">
         <v>20</v>
       </c>
@@ -2178,7 +2178,7 @@
         <f t="shared" si="0"/>
         <v>135.00000000000009</v>
       </c>
-      <c r="G13" s="65" t="s">
+      <c r="G13" s="38" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="36" t="s">
@@ -2199,7 +2199,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="66"/>
+      <c r="G14" s="39"/>
       <c r="H14" s="32"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
@@ -2216,7 +2216,7 @@
         <f>(D15-C15)*24*60 - E15</f>
         <v>0</v>
       </c>
-      <c r="G15" s="65"/>
+      <c r="G15" s="38"/>
       <c r="H15" s="36"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
@@ -2233,7 +2233,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="65"/>
+      <c r="G16" s="38"/>
       <c r="H16" s="36"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
@@ -2250,7 +2250,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="66"/>
+      <c r="G17" s="39"/>
       <c r="H17" s="32"/>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
@@ -2267,19 +2267,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="68"/>
+      <c r="G18" s="41"/>
       <c r="H18" s="32"/>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>1005.0000000000001</v>
@@ -2327,68 +2327,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="49" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="50">
+      <c r="G4" s="54">
         <v>43521</v>
       </c>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="51"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="54"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2432,7 +2432,7 @@
         <f>(D7-C7)*24*60 - E7</f>
         <v>90</v>
       </c>
-      <c r="G7" s="65" t="s">
+      <c r="G7" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="36" t="s">
@@ -2459,7 +2459,7 @@
         <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
         <v>49.999999999999986</v>
       </c>
-      <c r="G8" s="65" t="s">
+      <c r="G8" s="38" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="36" t="s">
@@ -2484,7 +2484,7 @@
         <f>(D9-C9)*24*60 - E9</f>
         <v>30.000000000000053</v>
       </c>
-      <c r="G9" s="65" t="s">
+      <c r="G9" s="38" t="s">
         <v>16</v>
       </c>
       <c r="H9" s="36" t="s">
@@ -2511,7 +2511,7 @@
         <f>(D10-C10)*24*60 - E10</f>
         <v>85.000000000000014</v>
       </c>
-      <c r="G10" s="65" t="s">
+      <c r="G10" s="38" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="36" t="s">
@@ -2538,7 +2538,7 @@
         <f>(D11-C11)*24*60 - E11</f>
         <v>120.00000000000006</v>
       </c>
-      <c r="G11" s="65" t="s">
+      <c r="G11" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H11" s="36"/>
@@ -2563,10 +2563,10 @@
         <f>(D12-C12)*24*60 - E12</f>
         <v>170.00000000000014</v>
       </c>
-      <c r="G12" s="59" t="s">
+      <c r="G12" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="57" t="s">
+      <c r="H12" s="61" t="s">
         <v>29</v>
       </c>
       <c r="I12" s="6"/>
@@ -2592,8 +2592,8 @@
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="G13" s="60"/>
-      <c r="H13" s="62"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="66"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
@@ -2617,8 +2617,8 @@
         <f t="shared" si="0"/>
         <v>260.00000000000011</v>
       </c>
-      <c r="G14" s="60"/>
-      <c r="H14" s="62"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="66"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
@@ -2640,8 +2640,8 @@
         <f>(D15-C15)*24*60 - E15</f>
         <v>75.000000000000057</v>
       </c>
-      <c r="G15" s="61"/>
-      <c r="H15" s="58"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="62"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
@@ -2657,7 +2657,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="65"/>
+      <c r="G16" s="38"/>
       <c r="H16" s="36"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
@@ -2674,7 +2674,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="66"/>
+      <c r="G17" s="39"/>
       <c r="H17" s="32"/>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
@@ -2691,19 +2691,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="68"/>
+      <c r="G18" s="41"/>
       <c r="H18" s="32"/>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>1380.0000000000005</v>
@@ -2751,68 +2751,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="49" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="50">
+      <c r="G4" s="54">
         <v>43527</v>
       </c>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="51"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="54"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2856,7 +2856,7 @@
         <f>(D7-C7)*24*60 - E7</f>
         <v>151.00000000000011</v>
       </c>
-      <c r="G7" s="65" t="s">
+      <c r="G7" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="36"/>
@@ -2879,7 +2879,7 @@
         <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
         <v>48.999999999999986</v>
       </c>
-      <c r="G8" s="65" t="s">
+      <c r="G8" s="38" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="36" t="s">
@@ -2906,7 +2906,7 @@
         <f>(D9-C9)*24*60 - E9</f>
         <v>130.00000000000009</v>
       </c>
-      <c r="G9" s="65" t="s">
+      <c r="G9" s="38" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="36" t="s">
@@ -2935,7 +2935,7 @@
         <f>(D10-C10)*24*60 - E10</f>
         <v>114.99999999999997</v>
       </c>
-      <c r="G10" s="65" t="s">
+      <c r="G10" s="38" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="36" t="s">
@@ -2962,7 +2962,7 @@
         <f>(D11-C11)*24*60 - E11</f>
         <v>54.999999999999929</v>
       </c>
-      <c r="G11" s="65" t="s">
+      <c r="G11" s="38" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="36" t="s">
@@ -2991,10 +2991,10 @@
         <f>(D12-C12)*24*60 - E12</f>
         <v>29.999999999999893</v>
       </c>
-      <c r="G12" s="59" t="s">
+      <c r="G12" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="59" t="s">
+      <c r="H12" s="63" t="s">
         <v>34</v>
       </c>
       <c r="I12" s="6"/>
@@ -3020,8 +3020,8 @@
         <f t="shared" si="0"/>
         <v>79.999999999999929</v>
       </c>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
@@ -3045,8 +3045,8 @@
         <f t="shared" si="0"/>
         <v>95.000000000000085</v>
       </c>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
@@ -3066,8 +3066,8 @@
         <f>(D15-C15)*24*60 - E15</f>
         <v>45</v>
       </c>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
@@ -3087,7 +3087,7 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="G16" s="65" t="s">
+      <c r="G16" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H16" s="35" t="s">
@@ -3112,7 +3112,7 @@
         <f t="shared" si="0"/>
         <v>120.00000000000006</v>
       </c>
-      <c r="G17" s="66" t="s">
+      <c r="G17" s="39" t="s">
         <v>16</v>
       </c>
       <c r="H17" s="32" t="s">
@@ -3133,19 +3133,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="68"/>
+      <c r="G18" s="41"/>
       <c r="H18" s="32"/>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>960.00000000000023</v>
@@ -3193,68 +3193,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="49" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="50">
+      <c r="G4" s="54">
         <v>43534</v>
       </c>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="51"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="54"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -3298,7 +3298,7 @@
         <f>(D7-C7)*24*60 - E7</f>
         <v>205.00000000000006</v>
       </c>
-      <c r="G7" s="65" t="s">
+      <c r="G7" s="38" t="s">
         <v>16</v>
       </c>
       <c r="H7" s="32" t="s">
@@ -3325,7 +3325,7 @@
         <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
         <v>59.999999999999943</v>
       </c>
-      <c r="G8" s="65" t="s">
+      <c r="G8" s="38" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="36" t="s">
@@ -3350,7 +3350,7 @@
         <f>(D9-C9)*24*60 - E9</f>
         <v>49.999999999999986</v>
       </c>
-      <c r="G9" s="65" t="s">
+      <c r="G9" s="38" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="36" t="s">
@@ -3377,7 +3377,7 @@
         <f>(D10-C10)*24*60 - E10</f>
         <v>140.00000000000006</v>
       </c>
-      <c r="G10" s="65" t="s">
+      <c r="G10" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="36"/>
@@ -3402,7 +3402,7 @@
         <f>(D11-C11)*24*60 - E11</f>
         <v>129.99999999999994</v>
       </c>
-      <c r="G11" s="65" t="s">
+      <c r="G11" s="38" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="36" t="s">
@@ -3431,7 +3431,7 @@
         <f>(D12-C12)*24*60 - E12</f>
         <v>190.00000000000017</v>
       </c>
-      <c r="G12" s="66" t="s">
+      <c r="G12" s="39" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -3456,7 +3456,7 @@
         <f t="shared" si="0"/>
         <v>35.000000000000036</v>
       </c>
-      <c r="G13" s="66" t="s">
+      <c r="G13" s="39" t="s">
         <v>40</v>
       </c>
       <c r="H13" s="6" t="s">
@@ -3481,10 +3481,10 @@
         <f t="shared" si="0"/>
         <v>150.00000000000011</v>
       </c>
-      <c r="G14" s="59" t="s">
+      <c r="G14" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="63" t="s">
+      <c r="H14" s="67" t="s">
         <v>37</v>
       </c>
       <c r="I14" s="6"/>
@@ -3508,8 +3508,8 @@
         <f>(D15-C15)*24*60 - E15</f>
         <v>94.999999999999986</v>
       </c>
-      <c r="G15" s="61"/>
-      <c r="H15" s="64"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="68"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
@@ -3531,7 +3531,7 @@
         <f t="shared" si="0"/>
         <v>59.999999999999744</v>
       </c>
-      <c r="G16" s="65" t="s">
+      <c r="G16" s="38" t="s">
         <v>16</v>
       </c>
       <c r="H16" s="36" t="s">
@@ -3554,7 +3554,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="66"/>
+      <c r="G17" s="39"/>
       <c r="H17" s="32"/>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
@@ -3571,19 +3571,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="68"/>
+      <c r="G18" s="41"/>
       <c r="H18" s="32"/>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>1115</v>
@@ -3614,7 +3614,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4F9FF2-393D-4BE8-8309-82E6CF37137A}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3631,68 +3633,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="49" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="50">
+      <c r="G4" s="54">
         <v>43541</v>
       </c>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="51"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="54"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -3736,7 +3738,7 @@
         <f>(D7-C7)*24*60 - E7</f>
         <v>90</v>
       </c>
-      <c r="G7" s="65" t="s">
+      <c r="G7" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="32" t="s">
@@ -3763,7 +3765,7 @@
         <f t="shared" ref="F8:F18" si="0">(D8-C8)*24*60 - E8</f>
         <v>20.000000000000249</v>
       </c>
-      <c r="G8" s="65" t="s">
+      <c r="G8" s="38" t="s">
         <v>40</v>
       </c>
       <c r="H8" s="36" t="s">
@@ -3790,7 +3792,7 @@
         <f>(D9-C9)*24*60 - E9</f>
         <v>84.999999999999858</v>
       </c>
-      <c r="G9" s="65" t="s">
+      <c r="G9" s="38" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="36" t="s">
@@ -3817,10 +3819,10 @@
         <f>(D10-C10)*24*60 - E10</f>
         <v>30.000000000000053</v>
       </c>
-      <c r="G10" s="59" t="s">
+      <c r="G10" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="63" t="s">
+      <c r="H10" s="67" t="s">
         <v>38</v>
       </c>
       <c r="I10" s="6"/>
@@ -3844,8 +3846,8 @@
         <f>(D11-C11)*24*60 - E11</f>
         <v>20.000000000000089</v>
       </c>
-      <c r="G11" s="61"/>
-      <c r="H11" s="64"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="68"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
@@ -3859,16 +3861,18 @@
       <c r="C12" s="8">
         <v>0.52430555555555558</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="8">
+        <v>0.56944444444444442</v>
+      </c>
       <c r="E12" s="6"/>
       <c r="F12" s="5">
         <f>(D12-C12)*24*60 - E12</f>
-        <v>-755</v>
-      </c>
-      <c r="G12" s="59" t="s">
+        <v>64.999999999999929</v>
+      </c>
+      <c r="G12" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="63" t="s">
+      <c r="H12" s="67" t="s">
         <v>43</v>
       </c>
       <c r="I12" s="6"/>
@@ -3878,16 +3882,20 @@
       <c r="A13" s="9">
         <v>7</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="7">
+        <v>43541</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.70138888888888884</v>
+      </c>
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
       <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="61"/>
-      <c r="H13" s="64"/>
+        <v>-1009.9999999999999</v>
+      </c>
+      <c r="G13" s="65"/>
+      <c r="H13" s="68"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
@@ -3903,7 +3911,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="65"/>
+      <c r="G14" s="38"/>
       <c r="H14" s="35"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
@@ -3920,7 +3928,7 @@
         <f>(D15-C15)*24*60 - E15</f>
         <v>0</v>
       </c>
-      <c r="G15" s="65"/>
+      <c r="G15" s="38"/>
       <c r="H15" s="35"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
@@ -3937,7 +3945,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="65"/>
+      <c r="G16" s="38"/>
       <c r="H16" s="36"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
@@ -3954,7 +3962,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="66"/>
+      <c r="G17" s="39"/>
       <c r="H17" s="32"/>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
@@ -3971,22 +3979,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="68"/>
+      <c r="G18" s="41"/>
       <c r="H18" s="32"/>
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>-509.99999999999977</v>
+        <v>-699.99999999999977</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>

</xml_diff>

<commit_message>
Razor Pages 1.7 - Add a new field
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399D54F1-3DFC-4D6E-A063-22FFFDCEA195}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B2AFCB-27EB-4D10-93A3-ACB8A5158289}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3615,7 +3615,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3886,13 +3886,15 @@
         <v>43541</v>
       </c>
       <c r="C13" s="8">
-        <v>0.70138888888888884</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D13" s="8"/>
-      <c r="E13" s="6"/>
+      <c r="E13" s="6">
+        <v>15</v>
+      </c>
       <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>-1009.9999999999999</v>
+        <v>-1215</v>
       </c>
       <c r="G13" s="65"/>
       <c r="H13" s="68"/>
@@ -3994,7 +3996,7 @@
       <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>-699.99999999999977</v>
+        <v>-904.99999999999977</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>

</xml_diff>

<commit_message>
Razor Pages 1.8 - Add validation
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B2AFCB-27EB-4D10-93A3-ACB8A5158289}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF62762-582F-4749-AA06-7132538186DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="44">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -164,10 +164,10 @@
     <t>Helping others with homework</t>
   </si>
   <si>
-    <t>Prep</t>
-  </si>
-  <si>
     <t>Completing "Get started with Razor pages" project</t>
+  </si>
+  <si>
+    <t>Completing "Razor Pages with EF Core"</t>
   </si>
 </sst>
 </file>
@@ -3615,7 +3615,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3672,7 +3672,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="54">
-        <v>43541</v>
+        <v>43542</v>
       </c>
       <c r="H4" s="54"/>
       <c r="I4" s="54"/>
@@ -3870,10 +3870,10 @@
         <v>64.999999999999929</v>
       </c>
       <c r="G12" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="67" t="s">
         <v>42</v>
-      </c>
-      <c r="H12" s="67" t="s">
-        <v>43</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
@@ -3888,17 +3888,21 @@
       <c r="C13" s="8">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="8">
+        <v>0.94097222222222221</v>
+      </c>
       <c r="E13" s="6">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>-1215</v>
+        <v>124.99999999999994</v>
       </c>
       <c r="G13" s="65"/>
       <c r="H13" s="68"/>
-      <c r="I13" s="6"/>
+      <c r="I13" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3913,8 +3917,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="38"/>
-      <c r="H14" s="35"/>
+      <c r="G14" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>43</v>
+      </c>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
@@ -3996,7 +4004,7 @@
       <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>-904.99999999999977</v>
+        <v>435.00000000000011</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>

</xml_diff>

<commit_message>
Razor Pages 2.1 - Get Started
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AC7B90-90E4-44CD-B127-4CD810C138CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C8F2E3-197E-4739-A8BB-26E2C43673DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -734,6 +734,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3615,7 +3618,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3910,17 +3913,21 @@
         <v>8</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="8">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.99930555555555556</v>
+      </c>
       <c r="E14" s="6"/>
       <c r="F14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="38" t="s">
+        <v>29.000000000000057</v>
+      </c>
+      <c r="G14" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="35" t="s">
+      <c r="H14" s="67" t="s">
         <v>43</v>
       </c>
       <c r="I14" s="6"/>
@@ -3931,15 +3938,21 @@
         <v>9</v>
       </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="6"/>
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="8">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="E15" s="6">
+        <v>10</v>
+      </c>
       <c r="F15" s="5">
         <f>(D15-C15)*24*60 - E15</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="38"/>
-      <c r="H15" s="35"/>
+        <v>66</v>
+      </c>
+      <c r="G15" s="64"/>
+      <c r="H15" s="69"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
@@ -3955,8 +3968,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="38"/>
-      <c r="H16" s="36"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="68"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
@@ -4004,7 +4017,7 @@
       <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>435.00000000000011</v>
+        <v>530.00000000000023</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>
@@ -4012,7 +4025,7 @@
       <c r="J19" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
@@ -4024,6 +4037,8 @@
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="H12:H13"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="H14:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Razor Pages 2.2 CRUD + fix
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C8F2E3-197E-4739-A8BB-26E2C43673DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7CD038-4395-47A2-A140-82FB7AA363EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3618,7 +3618,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3961,12 +3961,14 @@
         <v>10</v>
       </c>
       <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
+      <c r="C16" s="8">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D16" s="8"/>
       <c r="E16" s="6"/>
       <c r="F16" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-735</v>
       </c>
       <c r="G16" s="65"/>
       <c r="H16" s="68"/>
@@ -4017,7 +4019,7 @@
       <c r="E19" s="46"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>530.00000000000023</v>
+        <v>-204.99999999999977</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>

</xml_diff>

<commit_message>
Razor Pages 2.3 - Sort, Filter, Paging
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2636258E-AB20-4418-A12D-85BB3D4CC288}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D2E0F1-980B-4295-822F-83C846BDD425}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3632,7 +3632,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14:H17"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3996,12 +3996,16 @@
         <v>11</v>
       </c>
       <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8">
+        <v>0.82291666666666663</v>
+      </c>
       <c r="D17" s="8"/>
-      <c r="E17" s="6"/>
+      <c r="E17" s="6">
+        <v>15</v>
+      </c>
       <c r="F17" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1200</v>
       </c>
       <c r="G17" s="66"/>
       <c r="H17" s="72"/>
@@ -4035,7 +4039,7 @@
       <c r="E19" s="47"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>755.00000000000023</v>
+        <v>-444.99999999999977</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>

</xml_diff>

<commit_message>
Razor pages 2.7 - Update Related Data
</commit_message>
<xml_diff>
--- a/Galoyan_Time_recording_log.xlsx
+++ b/Galoyan_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\source\repos\ISA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08DEC43-CF63-4FE9-91B7-26FC84845963}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E53BCD5-FCB4-421E-8BB6-D0D6338B54DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3632,7 +3632,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3951,7 +3951,9 @@
       <c r="A15" s="9">
         <v>9</v>
       </c>
-      <c r="B15" s="7"/>
+      <c r="B15" s="7">
+        <v>43542</v>
+      </c>
       <c r="C15" s="8">
         <v>0</v>
       </c>
@@ -3999,13 +4001,15 @@
       <c r="C17" s="8">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D17" s="8"/>
+      <c r="D17" s="8">
+        <v>0.99305555555555547</v>
+      </c>
       <c r="E17" s="6">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="0"/>
-        <v>-1200</v>
+        <v>209.99999999999994</v>
       </c>
       <c r="G17" s="66"/>
       <c r="H17" s="72"/>
@@ -4039,7 +4043,7 @@
       <c r="E19" s="47"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>-444.99999999999977</v>
+        <v>965.00000000000023</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>

</xml_diff>